<commit_message>
assigned herlev hovedgade as master controller. is communicating with (to) kas sc for level and current cycle second
</commit_message>
<xml_diff>
--- a/Vissim/o3_roskildevej-herlevsygehus/Static_schedules.xlsx
+++ b/Vissim/o3_roskildevej-herlevsygehus/Static_schedules.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="9375" windowHeight="6090" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="9375" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mileparken" sheetId="1" r:id="rId1"/>
@@ -1384,7 +1384,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CC7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BR8" sqref="BR8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2130,18 +2133,18 @@
       <c r="BM7" s="5"/>
       <c r="BN7" s="5"/>
       <c r="BO7" s="5"/>
-      <c r="BP7" s="5"/>
-      <c r="BQ7" s="5"/>
-      <c r="BR7" s="5"/>
-      <c r="BS7" s="5"/>
-      <c r="BT7" s="5"/>
-      <c r="BU7" s="5"/>
+      <c r="BP7" s="4"/>
+      <c r="BQ7" s="4"/>
+      <c r="BR7" s="2"/>
+      <c r="BS7" s="2"/>
+      <c r="BT7" s="2"/>
+      <c r="BU7" s="2"/>
       <c r="BV7" s="2"/>
       <c r="BW7" s="2"/>
-      <c r="BX7" s="2"/>
-      <c r="BY7" s="2"/>
-      <c r="BZ7" s="5"/>
-      <c r="CA7" s="5"/>
+      <c r="BX7" s="3"/>
+      <c r="BY7" s="3"/>
+      <c r="BZ7" s="3"/>
+      <c r="CA7" s="3"/>
       <c r="CB7" s="5"/>
       <c r="CC7" s="5"/>
     </row>
@@ -3184,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>